<commit_message>
tdf#167941 - Chart style file is not supported in OOXML
Implement chart style file export, beginning to use the document
model data rather than hard-coded text. Also add a simple test
that style data round-trips OOXML -> LO -> OOXML properly.

This uses oox structures in docmodel. That will be fixed in a
subsequent commit.

Change-Id: Icc0ef5b212cc32c8c84b51529bc4cf05ab54636c
Reviewed-on: https://gerrit.libreoffice.org/c/core/+/190586
Tested-by: Jenkins
Reviewed-by: Tomaž Vajngerl <quikee@gmail.com>
Reviewed-on: https://gerrit.libreoffice.org/c/core/+/195578
Tested-by: Jenkins CollaboraOffice <jenkinscollaboraoffice@gmail.com>
</commit_message>
<xml_diff>
--- a/chart2/qa/extras/data/xlsx/column-style.xlsx
+++ b/chart2/qa/extras/data/xlsx/column-style.xlsx
@@ -81,10 +81,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="123"/>
+      <c14:style val="136"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="23"/>
+      <c:style val="36"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -125,20 +125,6 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:spPr>
-            <a:pattFill prst="ltUpDiag">
-              <a:fgClr>
-                <a:schemeClr val="accent1"/>
-              </a:fgClr>
-              <a:bgClr>
-                <a:schemeClr val="lt1"/>
-              </a:bgClr>
-            </a:pattFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
@@ -313,18 +299,6 @@
     </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="accent1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="accent1"/>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -392,7 +366,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:defRPr sz="777" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0">
@@ -404,7 +378,7 @@
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9999" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="phClr">
             <a:lumMod val="60000"/>

</xml_diff>

<commit_message>
tdf#168472 - Chart round-trip MSO -> LO -> MSO broken
Follow-up to earlier commit for this bug, improving the handling of
cs:ST_StyleColorVal and adding CI testing for FontReference and StyleReference

Change-Id: If8c86b780de07c38dfd67e4ba6c7739935698a27
Reviewed-on: https://gerrit.libreoffice.org/c/core/+/191416
Tested-by: Jenkins
Reviewed-by: Tomaž Vajngerl <quikee@gmail.com>
</commit_message>
<xml_diff>
--- a/chart2/qa/extras/data/xlsx/column-style.xlsx
+++ b/chart2/qa/extras/data/xlsx/column-style.xlsx
@@ -361,9 +361,9 @@
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="214">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
+    <cs:fillRef idx="7"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="major">
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:defRPr sz="777" b="1" kern="1200"/>

</xml_diff>

<commit_message>
tdf#167941 - Chart color sequence OOXML import/export
Support import, storage, and export of OOXML chart color styles
(color sequence). In OOXML, chart color styles are in files such
as colors1.xml, and conform to the chartStyle schema. This commit
supports I/O of color styles, and provides supports storing them
in the chart document model. It does not include any features for
using or modifying the color styles, so at this point it has no
appreciable effect on users.

Change-Id: I5c02137ebf9c25e11951eea55c4c77fda35b0e80
Reviewed-on: https://gerrit.libreoffice.org/c/core/+/194998
Tested-by: Jenkins
Reviewed-by: Tomaž Vajngerl <quikee@gmail.com>
</commit_message>
<xml_diff>
--- a/chart2/qa/extras/data/xlsx/column-style.xlsx
+++ b/chart2/qa/extras/data/xlsx/column-style.xlsx
@@ -318,42 +318,8 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="acrossLinear" id="10">
+  <a:schemeClr val="dk2"/>
 </cs:colorStyle>
 </file>
 
@@ -542,7 +508,7 @@
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="x" size="11"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>

</xml_diff>

<commit_message>
Revert "tdf#167941 - Chart style file is not supported in OOXML"
This reverts commit 526287a4aa7fe06bcfaa8fedc26106bd1a87fc88.

Change-Id: Ie286dea0fb442ba7ce6b396d8ce13696bd3620ac
Reviewed-on: https://gerrit.libreoffice.org/c/core/+/197895
Reviewed-by: Tomaž Vajngerl <quikee@gmail.com>
Tested-by: Jenkins CollaboraOffice <jenkinscollaboraoffice@gmail.com>
</commit_message>
<xml_diff>
--- a/chart2/qa/extras/data/xlsx/column-style.xlsx
+++ b/chart2/qa/extras/data/xlsx/column-style.xlsx
@@ -81,10 +81,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="136"/>
+      <c14:style val="123"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="36"/>
+      <c:style val="23"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -125,6 +125,20 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:spPr>
+            <a:pattFill prst="ltUpDiag">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="lt1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
@@ -299,6 +313,18 @@
     </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent1"/>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -366,7 +392,7 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
-    <cs:defRPr sz="777" b="1" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0">
@@ -378,7 +404,7 @@
       <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9999" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="3175" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="phClr">
             <a:lumMod val="60000"/>

</xml_diff>